<commit_message>
fix: POD 500 error - PaymentCollection model issues
- Remove non-existent created_at column from PaymentCollection creation
- Check for existing payment before creating duplicate
- Use proper PaymentMethod enum instead of string
- Fix analytics endpoint to use 'timestamp' column (model has timestamp, not changed_at)
- Wrap notification calls in try-except to prevent failures

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/user_credentials.xlsx
+++ b/user_credentials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Py\Delivery-System-III\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457AA15F-7ACD-45AE-97FA-862F057C4BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACB8A65-1CF3-4A4B-83CB-25A4C463B980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Users" sheetId="1" r:id="rId1"/>
@@ -1459,7 +1459,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1471,6 +1471,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1505,16 +1513,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1817,8 +1828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5533,7 +5544,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6131,7 +6144,7 @@
       <c r="A21" t="s">
         <v>60</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>140</v>
       </c>
       <c r="C21" t="s">
@@ -8535,6 +8548,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B21" r:id="rId1" xr:uid="{AEED4462-59DB-45DB-8285-682C97EA1325}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>